<commit_message>
added hdfs directory to write max truss in flink
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -6318,7 +6318,7 @@
   <dimension ref="A1:AN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6789,8 +6789,14 @@
       <c r="C10">
         <v>146</v>
       </c>
+      <c r="D10">
+        <v>125</v>
+      </c>
       <c r="E10">
         <v>76</v>
+      </c>
+      <c r="F10">
+        <v>67</v>
       </c>
       <c r="O10" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
maxtrusswriting in flink last attempt
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="45">
   <si>
     <t>Flink</t>
   </si>
@@ -96,9 +96,6 @@
     <t>MaxTruss, bidirectionalWiki</t>
   </si>
   <si>
-    <t>Cores\StartK</t>
-  </si>
-  <si>
     <t>connectTruss</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   <si>
     <t>adsssf</t>
   </si>
+  <si>
+    <t>StartK</t>
+  </si>
 </sst>
 </file>
 
@@ -196,12 +196,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,13 +222,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5962,15 +5970,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>716280</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>108966</xdr:rowOff>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>2286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6318,7 +6326,7 @@
   <dimension ref="A1:AN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="L11" sqref="L11:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6331,7 +6339,7 @@
         <v>0</v>
       </c>
       <c r="AN1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
@@ -6698,19 +6706,19 @@
         <f>AVERAGE(X8:AB8)</f>
         <v>104.6</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="6">
         <v>102</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Y8" s="6">
         <v>105</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="6">
         <v>106</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AA8" s="6">
         <v>107</v>
       </c>
-      <c r="AB8" s="5">
+      <c r="AB8" s="6">
         <v>103</v>
       </c>
     </row>
@@ -6763,25 +6771,25 @@
         <f>AVERAGE(X9:AB9)</f>
         <v>86.6</v>
       </c>
-      <c r="X9" s="5">
+      <c r="X9" s="6">
         <v>88</v>
       </c>
-      <c r="Y9" s="5">
+      <c r="Y9" s="6">
         <v>85</v>
       </c>
-      <c r="Z9" s="5">
+      <c r="Z9" s="6">
         <v>86</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AA9" s="6">
         <v>89</v>
       </c>
-      <c r="AB9" s="5">
+      <c r="AB9" s="6">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>784</v>
@@ -6911,7 +6919,7 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="W16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="X16" s="2"/>
     </row>
@@ -6919,23 +6927,24 @@
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>21</v>
+      <c r="F17" s="7"/>
+      <c r="G17" t="s">
+        <v>24</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y17" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="Z17" s="2"/>
       <c r="AB17" s="2"/>
@@ -6945,13 +6954,20 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F18" s="2">
+        <v>40</v>
+      </c>
+      <c r="G18" s="2">
         <v>20</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>10</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
       <c r="V18" s="2">
         <v>1</v>
       </c>
@@ -6974,11 +6990,20 @@
       <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2">
-        <v>10</v>
+      <c r="E19" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="F19">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="G19">
+        <v>85</v>
+      </c>
+      <c r="H19">
+        <v>205</v>
+      </c>
+      <c r="I19">
+        <v>900</v>
       </c>
       <c r="V19" s="2">
         <v>2</v>
@@ -7002,7 +7027,21 @@
       <c r="B20">
         <v>1088</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>130</v>
+      </c>
+      <c r="G20">
+        <v>113</v>
+      </c>
+      <c r="H20">
+        <v>172</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3200</v>
+      </c>
       <c r="V20" s="2">
         <v>4</v>
       </c>
@@ -7037,11 +7076,11 @@
         <f t="shared" si="3"/>
         <v>7.0439770554493304</v>
       </c>
-      <c r="Y21" s="5">
+      <c r="Y21" s="6">
         <v>6</v>
       </c>
-      <c r="Z21" s="5"/>
-      <c r="AB21" s="5"/>
+      <c r="Z21" s="6"/>
+      <c r="AB21" s="6"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -7062,11 +7101,11 @@
         <f t="shared" si="3"/>
         <v>8.5080831408775985</v>
       </c>
-      <c r="Y22" s="5">
+      <c r="Y22" s="6">
         <v>8</v>
       </c>
-      <c r="Z22" s="5"/>
-      <c r="AB22" s="5"/>
+      <c r="Z22" s="6"/>
+      <c r="AB22" s="6"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -7087,7 +7126,7 @@
         <f t="shared" si="3"/>
         <v>9.669291338582676</v>
       </c>
-      <c r="Y23" s="5">
+      <c r="Y23" s="6">
         <v>10</v>
       </c>
     </row>
@@ -7103,7 +7142,7 @@
         <f t="shared" si="3"/>
         <v>9.5193798449612395</v>
       </c>
-      <c r="Y24" s="5">
+      <c r="Y24" s="6">
         <v>20</v>
       </c>
     </row>
@@ -7132,31 +7171,31 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="W27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <f>AVERAGE(1548,1580,1580)</f>
@@ -7186,16 +7225,16 @@
         <v>1</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y28" s="2"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <f>AVERAGE(22803,21663,20072)</f>
@@ -7235,7 +7274,7 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <f>AVERAGE(50133,49282,48157)</f>
@@ -7275,7 +7314,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <f>AVERAGE(2806,2635,2583)</f>
@@ -7315,7 +7354,7 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32">
         <f>AVERAGE(26,27,27)</f>
@@ -7352,11 +7391,11 @@
         <f t="shared" si="5"/>
         <v>0.85803474484256237</v>
       </c>
-      <c r="Y32" s="5"/>
+      <c r="Y32" s="6"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <f>SUM(B28:B32)</f>
@@ -7393,7 +7432,7 @@
         <f t="shared" si="5"/>
         <v>0.88246471226927248</v>
       </c>
-      <c r="Y33" s="5"/>
+      <c r="Y33" s="6"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="V34" s="2">
@@ -7407,7 +7446,7 @@
         <f t="shared" si="5"/>
         <v>0.89657980456026054</v>
       </c>
-      <c r="Y34" s="5"/>
+      <c r="Y34" s="6"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -7442,31 +7481,31 @@
         <f t="shared" si="5"/>
         <v>0.89495114006514664</v>
       </c>
-      <c r="Y35" s="5"/>
+      <c r="Y35" s="6"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37">
         <f>B28/B$33</f>
@@ -7495,7 +7534,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38">
         <f t="shared" ref="B38:G42" si="8">B29/B$33</f>
@@ -7524,7 +7563,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <f t="shared" si="8"/>
@@ -7553,7 +7592,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <f t="shared" si="8"/>
@@ -7582,7 +7621,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <f t="shared" si="8"/>
@@ -7611,7 +7650,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42">
         <f t="shared" si="8"/>
@@ -7663,28 +7702,29 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B50" s="5"/>
       <c r="C50">
         <v>8.5</v>
       </c>
@@ -7694,11 +7734,14 @@
       <c r="E50">
         <v>14.5</v>
       </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B51" s="5"/>
       <c r="C51">
         <v>9</v>
       </c>
@@ -7708,11 +7751,14 @@
       <c r="E51">
         <v>14.5</v>
       </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B52" s="5"/>
       <c r="C52">
         <v>1</v>
       </c>
@@ -7722,11 +7768,14 @@
       <c r="E52">
         <v>1.5</v>
       </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B53" s="5"/>
       <c r="C53">
         <v>0.02</v>
       </c>
@@ -7736,10 +7785,12 @@
       <c r="E53">
         <v>0.02</v>
       </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54">
         <f>SUM(B50:B53)</f>
@@ -7791,22 +7842,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -7869,7 +7920,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61" t="e">
         <f t="shared" ref="B61" si="13">B52/B$54</f>
@@ -7898,7 +7949,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" t="e">
         <f t="shared" ref="B62" si="14">B53/B$54</f>

</xml_diff>

<commit_message>
added latest data to benchmarks
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -230,7 +230,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -6326,7 +6326,7 @@
   <dimension ref="A1:AN62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L17"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7031,13 +7031,13 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="G20">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="H20">
-        <v>172</v>
+        <v>104</v>
       </c>
       <c r="I20" s="1">
         <v>3200</v>

</xml_diff>

<commit_message>
slides 1.0 and pdf
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <t>Flink</t>
   </si>
@@ -163,6 +163,9 @@
   <si>
     <t>sasdfsdfsdf</t>
   </si>
+  <si>
+    <t>Flink no write</t>
+  </si>
 </sst>
 </file>
 
@@ -278,16 +281,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US"/>
               <a:t>Flink vs Spark - scaling by #cores</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -312,7 +314,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1466,7 +1468,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -1499,7 +1501,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1537,7 +1539,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1584,20 +1586,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Runtime</a:t>
+                  <a:t>Runtime in seconds</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> in seconds</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1622,7 +1619,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1660,7 +1657,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1735,7 +1732,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1763,7 +1760,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1804,20 +1803,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Spark</a:t>
+              <a:t>Spark - scaling by #cores</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> - scaling by #cores</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1842,7 +1836,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -2451,7 +2445,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -2484,7 +2478,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -2522,7 +2516,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -2569,20 +2563,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Runtime</a:t>
+                  <a:t>Runtime in seconds</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> in seconds</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2607,7 +2596,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -2645,7 +2634,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -2704,7 +2693,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -2732,7 +2721,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2773,20 +2764,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Spark - runtime percentage</a:t>
+              <a:t>Spark - runtime percentage per program part and #cores </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> per program part and #cores </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2811,7 +2797,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -3266,7 +3252,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -3326,7 +3312,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -3369,7 +3355,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -3402,7 +3388,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3443,7 +3431,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -3476,7 +3464,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -3909,7 +3897,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -3942,7 +3930,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -3980,7 +3968,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -4028,7 +4016,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -4061,7 +4049,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -4099,7 +4087,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -4142,7 +4130,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -4175,7 +4163,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4216,7 +4206,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -4249,7 +4239,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -4525,7 +4515,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -4587,7 +4577,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -4630,7 +4620,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -4663,7 +4653,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4704,28 +4696,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Spark vs</a:t>
+              <a:t>Spark vs Flink - Max Truss runtimes</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Flink - </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Max</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Truss runtimes</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4750,7 +4729,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -4890,9 +4869,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -4903,7 +4880,7 @@
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5083,7 +5060,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5116,7 +5093,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -5154,7 +5131,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -5205,7 +5182,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5238,7 +5215,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -5270,7 +5247,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -5313,7 +5290,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -5346,7 +5323,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -5387,20 +5366,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Spark vs</a:t>
+              <a:t>Spark vs Flink - Truss runtimes</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Flink - Truss runtimes</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5425,7 +5399,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -5572,9 +5546,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -5585,7 +5557,7 @@
                         <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5777,7 +5749,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5810,7 +5782,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -5848,7 +5820,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -5899,7 +5871,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -5932,7 +5904,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -5964,7 +5936,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6007,7 +5979,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -6040,7 +6012,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6082,7 +6056,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6115,7 +6089,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -6549,7 +6523,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -6582,7 +6556,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -6620,7 +6594,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6668,7 +6642,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -6701,7 +6675,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -6739,7 +6713,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6782,7 +6756,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -6815,7 +6789,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -6856,20 +6832,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Flink - runtime percentage</a:t>
+              <a:t>Flink - runtime percentage per program part and #cores </a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> per program part and #cores </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6894,7 +6865,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -7271,7 +7242,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -7331,7 +7302,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -7374,7 +7345,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -7407,7 +7378,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -7449,20 +7422,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Flink </a:t>
+              <a:t>Flink - scaling by #cores</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>- scaling by #cores</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7487,7 +7455,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -8094,7 +8062,7 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -8127,7 +8095,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -8165,7 +8133,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -8212,20 +8180,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Runtime</a:t>
+                  <a:t>Runtime in seconds</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> in seconds</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -8250,7 +8213,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -8288,7 +8251,7 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -8347,7 +8310,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -8375,7 +8338,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Segoe UI Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -14982,8 +14947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AY19" sqref="AY19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15724,7 +15689,12 @@
       <c r="B21">
         <v>78262</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21">
+        <v>171</v>
+      </c>
       <c r="V21" s="2">
         <v>6</v>
       </c>

</xml_diff>